<commit_message>
Finish creating SQL tables
All scripts are written to create the tables, and have been run against the database.
</commit_message>
<xml_diff>
--- a/OTHER FILES/Schema.xlsx
+++ b/OTHER FILES/Schema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fmsek\source\repos\harvp\DnD\OTHER FILES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Subversion\DnDTermProject\DnD\OTHER FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304B641E-6F1B-4E37-A98A-889A812AB12D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6696990-1E1D-497A-930A-481A5A195B31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="2085" windowWidth="12165" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8388" yWindow="276" windowWidth="13692" windowHeight="11724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First Draft of Schemas" sheetId="11" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="133">
   <si>
     <t>S</t>
   </si>
@@ -232,9 +232,6 @@
     <t>Score</t>
   </si>
   <si>
-    <t>Abilities</t>
-  </si>
-  <si>
     <t>AbilityID</t>
   </si>
   <si>
@@ -382,12 +379,6 @@
     <t>MaxDexBonus</t>
   </si>
   <si>
-    <t>Gear</t>
-  </si>
-  <si>
-    <t>gearID</t>
-  </si>
-  <si>
     <t>Languages</t>
   </si>
   <si>
@@ -410,6 +401,39 @@
   </si>
   <si>
     <t>hitPointsHigher</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>equipmentID</t>
+  </si>
+  <si>
+    <t>equipmentName</t>
+  </si>
+  <si>
+    <t>equpmentDescription</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>Races</t>
+  </si>
+  <si>
+    <t>raceName</t>
+  </si>
+  <si>
+    <t>abilityScoreIncrease</t>
+  </si>
+  <si>
+    <t>raceDescription</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability </t>
   </si>
 </sst>
 </file>
@@ -731,22 +755,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D1AF5C-3EDA-45F0-875A-6AFA4051B374}">
   <dimension ref="B3:T84"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="2"/>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
@@ -767,7 +793,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>3</v>
@@ -793,8 +819,10 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C8" s="2"/>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
@@ -815,9 +843,9 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="D10" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>40</v>
@@ -856,14 +884,17 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
       <c r="D14" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>53</v>
@@ -872,7 +903,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -888,7 +919,7 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
     </row>
-    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -903,14 +934,17 @@
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D18" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>63</v>
@@ -919,7 +953,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="E19" s="2"/>
@@ -935,7 +969,7 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -949,53 +983,56 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
       <c r="D21" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M22" s="2" t="s">
+      <c r="N22" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="O22" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="O22" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="E23" s="2"/>
@@ -1011,10 +1048,12 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D24" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1028,14 +1067,14 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1049,7 +1088,7 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1066,31 +1105,34 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
       <c r="D27" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -1100,25 +1142,28 @@
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
       <c r="D30" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D31" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="E32" s="2"/>
@@ -1134,9 +1179,12 @@
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
       <c r="D33" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -1151,15 +1199,15 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D34" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1175,7 +1223,7 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1191,7 +1239,10 @@
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
       <c r="D37" s="2" t="s">
         <v>35</v>
       </c>
@@ -1204,7 +1255,7 @@
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D38" s="2" t="s">
         <v>19</v>
       </c>
@@ -1218,7 +1269,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -1234,7 +1285,7 @@
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -1249,7 +1300,10 @@
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
       <c r="D41" s="2" t="s">
         <v>52</v>
       </c>
@@ -1266,7 +1320,7 @@
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D42" s="2" t="s">
         <v>55</v>
       </c>
@@ -1283,7 +1337,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1297,7 +1351,7 @@
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -1308,7 +1362,10 @@
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
       <c r="D45" s="2" t="s">
         <v>59</v>
       </c>
@@ -1322,7 +1379,7 @@
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D46" s="2" t="s">
         <v>53</v>
       </c>
@@ -1336,13 +1393,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -1353,37 +1410,42 @@
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
       <c r="D49" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="2"/>
       <c r="D50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="C52" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D52" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>42</v>
@@ -1392,153 +1454,172 @@
         <v>50</v>
       </c>
       <c r="G53" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H53" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H53" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="2"/>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B56" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="D56" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D57" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>50</v>
       </c>
       <c r="G57" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H57" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H57" s="2" t="s">
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>131</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D59" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B60" s="2"/>
       <c r="D60" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="F60" s="2"/>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>11</v>
+      </c>
       <c r="D62" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B63" s="2"/>
       <c r="D63" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="G63" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="H63" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H63" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>11</v>
+      </c>
       <c r="D66" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B67" s="2"/>
       <c r="D67" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="G67" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G67" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="H67" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
+      <c r="C69" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D69" s="2" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D70" s="2" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="G70" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B72" s="2"/>
+      <c r="C72" t="s">
+        <v>11</v>
+      </c>
       <c r="D72" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D73" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>40</v>
@@ -1547,28 +1628,56 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>11</v>
+      </c>
       <c r="D75" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B76" s="2"/>
       <c r="D76" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F76" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G76" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D79" t="s">
+        <v>22</v>
+      </c>
+      <c r="E79" t="s">
+        <v>128</v>
+      </c>
+      <c r="F79" t="s">
+        <v>129</v>
+      </c>
+      <c r="G79" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B84" s="2"/>
       <c r="D84" s="2"/>
     </row>
@@ -1583,7 +1692,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1597,7 +1706,7 @@
       <selection activeCell="B14" sqref="B4:J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1611,9 +1720,9 @@
       <selection activeCell="C7" sqref="C7:K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:11" x14ac:dyDescent="0.3">
       <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1622,7 +1731,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>6</v>
       </c>
@@ -1641,7 +1750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1652,7 +1761,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1663,7 +1772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1687,17 +1796,17 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="32.28515625" customWidth="1"/>
+    <col min="10" max="10" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:12" x14ac:dyDescent="0.3">
       <c r="G5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1718,9 +1827,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
@@ -1732,7 +1841,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>17</v>
       </c>
@@ -1743,7 +1852,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>18</v>
       </c>
@@ -1757,7 +1866,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>19</v>
       </c>
@@ -1771,7 +1880,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>20</v>
       </c>
@@ -1785,7 +1894,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>21</v>
       </c>
@@ -1796,7 +1905,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>22</v>
       </c>
@@ -1810,7 +1919,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>23</v>
       </c>
@@ -1821,7 +1930,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>24</v>
       </c>
@@ -1832,7 +1941,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>25</v>
       </c>
@@ -1843,7 +1952,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>26</v>
       </c>
@@ -1863,18 +1972,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55841BD6-24D4-439D-B408-689EEA83816B}">
   <dimension ref="D4:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:12" x14ac:dyDescent="0.3">
       <c r="G4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1895,7 +2004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>19</v>
       </c>
@@ -1906,7 +2015,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>36</v>
       </c>
@@ -1917,7 +2026,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>37</v>
       </c>
@@ -1928,7 +2037,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>25</v>
       </c>
@@ -1939,29 +2048,29 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F18" t="s">
         <v>39</v>
       </c>
       <c r="L18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F20" t="s">
         <v>39</v>
       </c>
       <c r="L20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>52</v>
       </c>
@@ -1969,7 +2078,7 @@
         <v>38</v>
       </c>
       <c r="L22" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1983,7 +2092,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1995,7 +2104,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2009,9 +2118,9 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2027,9 +2136,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2045,7 +2154,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>